<commit_message>
PageUtility class added and implemented.
</commit_message>
<xml_diff>
--- a/7rmart/src/test/resources/TestData.xlsx
+++ b/7rmart/src/test/resources/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7620" firstSheet="2" activeTab="3"/>
+    <workbookView windowWidth="20490" windowHeight="7620" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>Username</t>
   </si>
@@ -74,9 +74,6 @@
   </si>
   <si>
     <t>12 B, Skyline, Kakkanad, Kochi</t>
-  </si>
-  <si>
-    <t>1 hour</t>
   </si>
   <si>
     <t>Rs. 100</t>
@@ -1381,7 +1378,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="4"/>
@@ -1420,11 +1417,11 @@
       <c r="C2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="4">
+        <v>42.5</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1452,12 +1449,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>